<commit_message>
chatbot funcionando - versão alpha
</commit_message>
<xml_diff>
--- a/data/matriculas.xlsx
+++ b/data/matriculas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe570407d8e87ac/Área de Trabalho/Data Science/Gen AI/projetos/chatbot-whatsapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="11_AD4D361C20488DEA4E38A0BF541B7A425ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A2D62FD-A463-4559-8AD9-F1B95AC60622}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_AD4D361C20488DEA4E38A0BF541B7A425ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DC49CE8-D5AA-4C0B-9921-BE1DF7C366F6}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>matricula</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Jean Paulo Kambourakis</t>
-  </si>
-  <si>
-    <t>Nanda Annanda Destro Torteli</t>
   </si>
 </sst>
 </file>
@@ -406,11 +403,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -558,14 +553,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>808110</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>